<commit_message>
update desciption of Tables ; add API for equip
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20364"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\10303\Desktop\程序实践\大作业\bighw-backend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\真·学习\大2下\_小学期\py\git bighw\bighw-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6890A5D-C3BA-431B-BEA8-4D618425D439}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C434E23-CA99-46C1-84B4-25C59DA6A767}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="1425" windowWidth="21600" windowHeight="11385" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1680" yWindow="1428" windowWidth="21600" windowHeight="11388" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
   <si>
     <t>username</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -76,10 +76,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>address</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -136,12 +132,6 @@
   </si>
   <si>
     <t>date</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>avaliable
-rented
-unavaliable</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -150,10 +140,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>lessor</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>equip_id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -175,6 +161,48 @@
   </si>
   <si>
     <t>accepted</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用于验证邮箱与session验证</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>租期结束时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>去哪领</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>student_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>学号，管理员看到</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>一般看到的是默认id(从1开始)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>有个默认的id从1开始</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>申请记录只会被admin删除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可租onsale
+已出租rented
+下架unavailable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>默认id从1开始</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -182,7 +210,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,6 +220,22 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color theme="1"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
@@ -218,11 +262,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -506,18 +552,19 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="5" width="12.25" customWidth="1"/>
-    <col min="6" max="6" width="18.125" customWidth="1"/>
-    <col min="7" max="8" width="15.75" customWidth="1"/>
-    <col min="9" max="9" width="19.625" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" customWidth="1"/>
+    <col min="4" max="5" width="12.21875" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" customWidth="1"/>
+    <col min="7" max="8" width="15.77734375" customWidth="1"/>
+    <col min="9" max="10" width="24.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -525,13 +572,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F1" t="s">
         <v>2</v>
@@ -540,13 +587,13 @@
         <v>3</v>
       </c>
       <c r="H1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -565,13 +612,22 @@
       <c r="G2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="I2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C3" s="3" t="s">
+        <v>37</v>
+      </c>
       <c r="F3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C4" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="F4" t="s">
         <v>10</v>
       </c>
@@ -585,49 +641,65 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{013A9874-B74F-455B-AC44-E6FB0D0B1476}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.625" customWidth="1"/>
+    <col min="1" max="1" width="11.21875" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
-        <v>13</v>
-      </c>
       <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
         <v>15</v>
       </c>
-      <c r="F1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>27</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -639,20 +711,20 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
         <v>17</v>
-      </c>
-      <c r="D1" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -663,28 +735,31 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABD63059-0B8A-4968-B24E-4CA29B145FDF}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.25" customWidth="1"/>
+    <col min="2" max="2" width="23.21875" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
-        <v>21</v>
-      </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -695,59 +770,71 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125788D2-CB5C-4C17-9457-4354C17ABF18}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView topLeftCell="B1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.75" customWidth="1"/>
-    <col min="2" max="2" width="12.625" customWidth="1"/>
+    <col min="1" max="1" width="10.77734375" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="11.875" customWidth="1"/>
+    <col min="4" max="4" width="11.88671875" customWidth="1"/>
+    <col min="5" max="5" width="13.77734375" customWidth="1"/>
+    <col min="7" max="7" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
         <v>30</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
         <v>31</v>
       </c>
-      <c r="H1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H4" t="s">
-        <v>34</v>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H6" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -761,48 +848,48 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.25" customWidth="1"/>
-    <col min="3" max="3" width="11.75" customWidth="1"/>
-    <col min="4" max="4" width="12.25" customWidth="1"/>
-    <col min="5" max="5" width="11.625" customWidth="1"/>
-    <col min="6" max="6" width="11.125" customWidth="1"/>
-    <col min="7" max="7" width="10.75" customWidth="1"/>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" customWidth="1"/>
+    <col min="7" max="7" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
-        <v>21</v>
-      </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" t="s">
-        <v>25</v>
-      </c>
       <c r="H1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F2" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add user_id lessor_id to all tables
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20364"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\真·学习\大2下\_小学期\py\git bighw\bighw-backend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\75993\Desktop\Python\homework\project\bighw-backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26ACA1B7-CCF2-42C6-BF13-84C21FE5012D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC23425F-92A3-49A6-80A4-E9CADF39AD1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="49">
   <si>
     <t>username</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -219,6 +219,14 @@
   </si>
   <si>
     <t>reject</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lessor_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user_id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -585,19 +593,19 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="A2" sqref="A2:F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="18.109375" customWidth="1"/>
-    <col min="4" max="5" width="12.21875" customWidth="1"/>
-    <col min="6" max="6" width="18.109375" customWidth="1"/>
-    <col min="7" max="8" width="15.77734375" customWidth="1"/>
-    <col min="9" max="10" width="24.88671875" customWidth="1"/>
+    <col min="3" max="3" width="18.125" customWidth="1"/>
+    <col min="4" max="5" width="12.25" customWidth="1"/>
+    <col min="6" max="6" width="18.125" customWidth="1"/>
+    <col min="7" max="8" width="15.75" customWidth="1"/>
+    <col min="9" max="10" width="24.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -626,7 +634,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -649,7 +657,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C3" s="3" t="s">
         <v>33</v>
       </c>
@@ -657,7 +665,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C4" s="3" t="s">
         <v>34</v>
       </c>
@@ -674,22 +682,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{013A9874-B74F-455B-AC44-E6FB0D0B1476}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.21875" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="10.44140625" customWidth="1"/>
-    <col min="6" max="6" width="15" customWidth="1"/>
-    <col min="7" max="7" width="17.21875" customWidth="1"/>
+    <col min="1" max="1" width="11.25" customWidth="1"/>
+    <col min="2" max="3" width="12.625" customWidth="1"/>
+    <col min="5" max="5" width="10.5" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
+    <col min="8" max="8" width="17.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -697,38 +705,44 @@
         <v>20</v>
       </c>
       <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>13</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" t="s">
+      <c r="I1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E2" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D3" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>35</v>
       </c>
@@ -748,9 +762,9 @@
       <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -767,17 +781,17 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E2" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E3" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E4" s="5" t="s">
         <v>46</v>
       </c>
@@ -791,20 +805,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABD63059-0B8A-4968-B24E-4CA29B145FDF}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="23.21875" customWidth="1"/>
+    <col min="2" max="2" width="23.25" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -816,6 +830,9 @@
       </c>
       <c r="D1" t="s">
         <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -826,76 +843,82 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125788D2-CB5C-4C17-9457-4354C17ABF18}">
-  <dimension ref="A1:H8"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView topLeftCell="B1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="17.109375" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.77734375" customWidth="1"/>
-    <col min="7" max="7" width="12.44140625" customWidth="1"/>
+    <col min="1" max="2" width="10.75" customWidth="1"/>
+    <col min="3" max="3" width="12.625" customWidth="1"/>
+    <col min="4" max="4" width="17.125" customWidth="1"/>
+    <col min="5" max="5" width="21.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.75" customWidth="1"/>
+    <col min="9" max="9" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" t="s">
         <v>42</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>22</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>20</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H2" s="4" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J2" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H3" s="5" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J3" s="5" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H4" s="5" t="s">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J4" s="5" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="H6" s="3" t="s">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J6" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
         <v>38</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>39</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>40</v>
       </c>
     </row>
@@ -908,23 +931,23 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3986A193-9E1D-451D-A862-964016297726}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" customWidth="1"/>
-    <col min="7" max="7" width="10.77734375" customWidth="1"/>
+    <col min="3" max="4" width="11.75" customWidth="1"/>
+    <col min="5" max="6" width="12.25" customWidth="1"/>
+    <col min="7" max="7" width="11.625" customWidth="1"/>
+    <col min="8" max="8" width="11.125" customWidth="1"/>
+    <col min="9" max="9" width="10.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -935,23 +958,29 @@
         <v>20</v>
       </c>
       <c r="D1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>22</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F2" s="1" t="s">
+    <row r="2" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H2" s="1" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update RegisterApp ; add MessageApp
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\真·学习\大2下\_小学期\py\git bighw\bighw-backend\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\真·学习\大2下\_小学期\py\大作业\czlProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26ACA1B7-CCF2-42C6-BF13-84C21FE5012D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2BFB6C8-163B-45BA-804A-C8E88367E225}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="sale_req" sheetId="5" r:id="rId4"/>
     <sheet name="rent_req" sheetId="6" r:id="rId5"/>
     <sheet name="rent_info" sheetId="3" r:id="rId6"/>
+    <sheet name="message" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="61">
   <si>
     <t>username</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -219,6 +220,62 @@
   </si>
   <si>
     <t>reject</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>all表示是系统日志</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user表示是给user的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lessor表示给lessor的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>title</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消息标题</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消息内容</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>消息发出时间</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>数字,表示用户id，</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>为0时表示是系统日志</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>to_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>from_id</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -226,7 +283,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -272,6 +329,21 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -293,7 +365,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -302,6 +374,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -828,7 +903,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{125788D2-CB5C-4C17-9457-4354C17ABF18}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView topLeftCell="B22" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
@@ -959,4 +1034,89 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47BBCCAE-BC4A-46B7-96B3-E715C7393859}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="22.8" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="1" width="15.21875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="17.21875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="12.77734375" style="7" customWidth="1"/>
+    <col min="9" max="9" width="12.88671875" style="7" customWidth="1"/>
+    <col min="10" max="10" width="13" style="7" customWidth="1"/>
+    <col min="11" max="16384" width="8.88671875" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="5" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
+      <c r="A3" s="8"/>
+    </row>
+    <row r="4" spans="1:6" s="5" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="5" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="5" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="5" customFormat="1" ht="11.4" x14ac:dyDescent="0.2"/>
+    <row r="8" spans="1:6" s="5" customFormat="1" ht="11.4" x14ac:dyDescent="0.2"/>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add api for message
</commit_message>
<xml_diff>
--- a/tables.xlsx
+++ b/tables.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\真·学习\大2下\_小学期\py\大作业\czlProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2BFB6C8-163B-45BA-804A-C8E88367E225}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44C6522-7D8C-4FED-9EA8-A36AB5A39C42}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="63">
   <si>
     <t>username</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -227,10 +227,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>all表示是系统日志</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>user表示是给user的</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -276,6 +272,18 @@
   </si>
   <si>
     <t>from_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sys表示是系统日志</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>为0时表示是系统发出的</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>包括日期和时间</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1041,13 +1049,13 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22.8" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="15.21875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" style="7" customWidth="1"/>
     <col min="3" max="3" width="17.21875" style="7" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" style="7" customWidth="1"/>
     <col min="5" max="5" width="12.44140625" style="7" customWidth="1"/>
@@ -1064,19 +1072,19 @@
         <v>47</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="5" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
@@ -1084,32 +1092,41 @@
     </row>
     <row r="4" spans="1:6" s="5" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>48</v>
+        <v>60</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>56</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="5" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>61</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="5" customFormat="1" ht="11.4" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="5" customFormat="1" ht="11.4" x14ac:dyDescent="0.2"/>

</xml_diff>